<commit_message>
added security rule for jenkins
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thinkaheadit-my.sharepoint.com/personal/amandeep_singh_ahead_com/Documents/Documents/Learning/Terraform Study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_F25DC773A252ABDACC10486D611C79325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90DAAA57-4173-4A4F-90AA-101F3C7DDFD0}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC10486D611C79325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5367818-5C77-41F5-9A69-70633D06D913}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,6 +98,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -363,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,7 +433,7 @@
         <v>36</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C7" si="0">B5/200*100</f>
+        <f t="shared" ref="C5:C10" si="0">B5/200*100</f>
         <v>18</v>
       </c>
     </row>
@@ -455,6 +459,42 @@
       <c r="C7">
         <f t="shared" si="0"/>
         <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>45789</v>
+      </c>
+      <c r="B8">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>45790</v>
+      </c>
+      <c r="B9">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45793</v>
+      </c>
+      <c r="B10">
+        <v>58</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>28.999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added key vault terraform
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thinkaheadit-my.sharepoint.com/personal/amandeep_singh_ahead_com/Documents/Documents/Learning/Terraform Study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC10486D611C79325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5367818-5C77-41F5-9A69-70633D06D913}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="11_F25DC773A252ABDACC10486D611C79325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12336123-1947-44B2-829E-5FEC68700C51}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,7 +433,7 @@
         <v>36</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C10" si="0">B5/200*100</f>
+        <f t="shared" ref="C5:C11" si="0">B5/200*100</f>
         <v>18</v>
       </c>
     </row>
@@ -495,6 +495,18 @@
       <c r="C10">
         <f t="shared" si="0"/>
         <v>28.999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>45794</v>
+      </c>
+      <c r="B11">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved vm password to key vault
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thinkaheadit-my.sharepoint.com/personal/amandeep_singh_ahead_com/Documents/Documents/Learning/Terraform Study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_F25DC773A252ABDACC10486D611C79325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12336123-1947-44B2-829E-5FEC68700C51}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_F25DC773A252ABDACC10486D611C79325ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E2714F2-752A-4E0C-90FA-C48A09524C6C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,7 +433,7 @@
         <v>36</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C11" si="0">B5/200*100</f>
+        <f t="shared" ref="C5:C12" si="0">B5/200*100</f>
         <v>18</v>
       </c>
     </row>
@@ -507,6 +507,18 @@
       <c r="C11">
         <f t="shared" si="0"/>
         <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>45795</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>